<commit_message>
fixed some python bugs
</commit_message>
<xml_diff>
--- a/Assembler/Microcode.xlsx
+++ b/Assembler/Microcode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t xml:space="preserve">MDRen IRin WRsel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFout Yin Y=B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFin DSTsel Yout END</t>
   </si>
 </sst>
 </file>
@@ -62,6 +71,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,17 +131,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -260,7 +274,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -295,153 +309,171 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="0"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="23.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="0"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0"/>
-      <c r="C4" s="0" t="n">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="0"/>
-      <c r="E4" s="0"/>
-      <c r="F4" s="0" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
-      <c r="I4" s="0"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
-      <c r="F5" s="0"/>
-      <c r="G5" s="0"/>
-      <c r="H5" s="0"/>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
-      <c r="G9" s="0"/>
-      <c r="H9" s="0"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-      <c r="G11" s="0"/>
-      <c r="H11" s="0"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-      <c r="G12" s="0"/>
-      <c r="H12" s="0"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="0"/>
-      <c r="H13" s="0"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="0"/>
-      <c r="H14" s="0"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
-      <c r="G16" s="0"/>
-      <c r="H16" s="0"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
rewrote the python code
</commit_message>
<xml_diff>
--- a/Assembler/Microcode.xlsx
+++ b/Assembler/Microcode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -55,7 +55,10 @@
     <t xml:space="preserve">RFout Yin Y=B</t>
   </si>
   <si>
-    <t xml:space="preserve">RFin DSTsel Yout END</t>
+    <t xml:space="preserve">RFin DSTsel Yout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCend</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,7 +356,7 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="n">
@@ -386,11 +389,20 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>5</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>

</xml_diff>

<commit_message>
solved the logic problem
</commit_message>
<xml_diff>
--- a/Assembler/Microcode.xlsx
+++ b/Assembler/Microcode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -59,6 +59,27 @@
   </si>
   <si>
     <t xml:space="preserve">TCend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCout PCinc MARin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFin DSTsel MDRen WRsel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFout Xin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFout DSTsel Yin ADD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
   </si>
 </sst>
 </file>
@@ -134,7 +155,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -149,6 +170,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -274,40 +303,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.39"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -356,7 +388,7 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="n">
@@ -416,76 +448,154 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>4</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>5</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>6</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>3</v>
+      </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>4</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>5</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
+    </row>
+    <row r="17" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added JMP, fixed conditions
</commit_message>
<xml_diff>
--- a/Assembler/Microcode.xlsx
+++ b/Assembler/Microcode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -80,6 +80,33 @@
   </si>
   <si>
     <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSTsel RFout Xin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB Yin RFout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCout MARin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDRen WRsel PCin</t>
   </si>
 </sst>
 </file>
@@ -155,7 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -164,12 +191,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -303,299 +350,421 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="24.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.39"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="23.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="n">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="n">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="n">
+      <c r="B5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="n">
+      <c r="B6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="n">
+      <c r="B7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="n">
+      <c r="B11" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3" t="n">
+      <c r="B14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3" t="n">
+      <c r="B15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3" t="n">
+      <c r="B16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="10" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="19" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1"/>
+      <c r="F31" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>